<commit_message>
Add supply and confirmation result to contact summary
</commit_message>
<xml_diff>
--- a/templates/stock_supply.xlsx
+++ b/templates/stock_supply.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Documents/Work/medic/app-services-team/stock-monitoring/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24004395-792B-484E-9108-7EEA1B61DA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C8F60E-6DC9-F84D-94D8-E6B618B2E587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="3300" windowWidth="29340" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="1620" windowWidth="29340" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -603,11 +603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -623,7 +623,7 @@
     <col min="9" max="16384" width="11.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -651,8 +651,18 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -670,8 +680,18 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -685,7 +705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -696,7 +716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -710,8 +730,18 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -722,7 +752,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
@@ -734,8 +764,18 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -749,8 +789,18 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>40</v>
       </c>
@@ -764,7 +814,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -775,7 +825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -787,8 +837,18 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -800,8 +860,18 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -815,7 +885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
@@ -831,8 +901,18 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -840,7 +920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -851,7 +931,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
@@ -863,8 +943,18 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>9</v>
       </c>
@@ -880,8 +970,18 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -893,6 +993,16 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Add need_signed_of to template
</commit_message>
<xml_diff>
--- a/templates/stock_supply.xlsx
+++ b/templates/stock_supply.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Documents/Work/medic/app-services-team/stock-monitoring/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romuald/Developer/medic/cht-stock-monitoring-workflow/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C8F60E-6DC9-F84D-94D8-E6B618B2E587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2B7388-EB34-B54C-8A6D-3E427A8792C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1620" windowWidth="29340" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>type</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>list_name</t>
+  </si>
+  <si>
+    <t>needs_signoff</t>
   </si>
 </sst>
 </file>
@@ -603,11 +606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1003,6 +1006,17 @@
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>